<commit_message>
added to and reshaped uds_codes.xlsx
</commit_message>
<xml_diff>
--- a/lookup/uds_codes.xlsx
+++ b/lookup/uds_codes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/josephking/Documents/Projects/demonstrations/uds_logs/lookup/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B55F72B3-445A-2741-8F4E-32F07A7C7ECD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C5B57B5-C673-B740-B293-A94A95638308}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14740" yWindow="6720" windowWidth="53900" windowHeight="27220" activeTab="1" xr2:uid="{F014B03A-22FC-3846-822F-66D5E0AB7371}"/>
+    <workbookView xWindow="30840" yWindow="19800" windowWidth="25480" windowHeight="20520" activeTab="1" xr2:uid="{F014B03A-22FC-3846-822F-66D5E0AB7371}"/>
   </bookViews>
   <sheets>
     <sheet name="services" sheetId="2" r:id="rId1"/>
@@ -3027,8 +3027,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A03570A-127B-3341-B38D-DB2BAB5CD826}">
   <dimension ref="A1:C84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C68" sqref="C68"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3044,7 +3044,7 @@
         <v>83</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>121</v>
+        <v>164</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>84</v>

</xml_diff>

<commit_message>
small change to uds_codes.xlsx
</commit_message>
<xml_diff>
--- a/lookup/uds_codes.xlsx
+++ b/lookup/uds_codes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/josephking/Documents/Projects/demonstrations/uds_logs/lookup/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C5B57B5-C673-B740-B293-A94A95638308}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3286F466-192E-1745-A007-3F16EA6DDDCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30840" yWindow="19800" windowWidth="25480" windowHeight="20520" activeTab="1" xr2:uid="{F014B03A-22FC-3846-822F-66D5E0AB7371}"/>
+    <workbookView xWindow="40700" yWindow="14800" windowWidth="25480" windowHeight="20520" activeTab="1" xr2:uid="{F014B03A-22FC-3846-822F-66D5E0AB7371}"/>
   </bookViews>
   <sheets>
     <sheet name="services" sheetId="2" r:id="rId1"/>
@@ -1498,7 +1498,7 @@
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
+      <selection pane="bottomLeft" activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3027,8 +3027,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A03570A-127B-3341-B38D-DB2BAB5CD826}">
   <dimension ref="A1:C84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
added check that DB values are unique on Code and Type
</commit_message>
<xml_diff>
--- a/lookup/uds_codes.xlsx
+++ b/lookup/uds_codes.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/josephking/Documents/Projects/demonstrations/uds_logs/lookup/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3286F466-192E-1745-A007-3F16EA6DDDCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C54D0621-F60C-2044-A9AB-7C4AA97EB5A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40700" yWindow="14800" windowWidth="25480" windowHeight="20520" activeTab="1" xr2:uid="{F014B03A-22FC-3846-822F-66D5E0AB7371}"/>
+    <workbookView xWindow="30640" yWindow="8580" windowWidth="35780" windowHeight="26400" activeTab="1" xr2:uid="{F014B03A-22FC-3846-822F-66D5E0AB7371}"/>
   </bookViews>
   <sheets>
     <sheet name="services" sheetId="2" r:id="rId1"/>
-    <sheet name="nrc" sheetId="3" r:id="rId2"/>
+    <sheet name="service_gpt" sheetId="5" r:id="rId2"/>
+    <sheet name="nrc" sheetId="3" r:id="rId3"/>
+    <sheet name="nrc_gpt" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1065" uniqueCount="469">
   <si>
     <t>0x10</t>
   </si>
@@ -693,9 +695,6 @@
     <t>0xFF</t>
   </si>
   <si>
-    <t xml:space="preserve"> This NRC shall not be used in a negative response message. This positiveResponse parameter value is reserved for server internal implementation.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> ISO Reserved.  This range of values is reserved for future definition by ISO 14229 Standard.</t>
   </si>
   <si>
@@ -1084,13 +1083,1792 @@
   </si>
   <si>
     <t>This NRC indicates that the requested action will not be taken because the server does not support the requested service in the session currently active. This NRC shall only be used when the requested service is known to be supported in another session, otherwise response code Service Not Supported shall be used.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> This positive response parameter value is reserved for server internal implementation.</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>Explanation</t>
+  </si>
+  <si>
+    <r>
+      <t>General Reject</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: The server does not support the requested service or sub-function.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Service Not Supported</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: The requested service is not supported by the server.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Service Not Supported in Active Session</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: The requested service is not supported in the current diagnostic session.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Sub-Function Not Supported</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: The requested sub-function is not supported by the server.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Incorrect Message Length or Invalid Format</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: The format or length of the request message is incorrect.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Response Too Long</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: The response generated by the server is too large.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Busy Repeat Request</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: The server is currently busy processing another request and asks the client to repeat the request.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Conditions Not Correct</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: The server conditions are not correct for executing the requested service.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Request Sequence Error</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: The order of requests sent by the client is incorrect.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>No Response from Subnet Component</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: There was no response from a required component on the subnet.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Service Not Supported in Current Active Diagnostic Session</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: The service is not available in the active session.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Voltage Too High</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: The voltage level is too high for the service to be performed.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Voltage Too Low</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: The voltage level is too low for the service to be performed.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Programming Failure</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: A failure occurred during programming.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Wrong Block Sequence Counter</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: The block sequence counter does not match the expected value, likely due to a communication issue.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Request Out of Range</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: The requested action or parameter is out of the valid range.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Security Access Denied</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: The server has denied access to the requested service, possibly due to a security violation.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Exceeded Number of Attempts</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: The client has exceeded the allowed number of attempts to access a service or feature.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Time Delay Not Expired</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: A time delay requirement has not expired, and the request cannot be processed yet.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Service Already in Progress</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: The service is already being processed, and no additional requests can be handled.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Request Correctly Received - Response Pending</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: The server received the request correctly, but a delay is needed for the response.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Sub-Function Not Supported in Current Session</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: The sub-function requested is not available in the current diagnostic session.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>General Programming Failure</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: A general failure occurred during programming.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>General Programming Failure</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (alternate): Some systems use 0x37 as a variant of 0x36, also indicating a programming failure.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Data Mismatch</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: The data provided does not match the expected format or content.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Request Sequence Error</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (alternate): Similar to 0x20, used in some systems to denote incorrect request sequence.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Request Sequence Error (alternate)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Some systems use this code similarly to 0x39, as a sequence error.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Pending Programming</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Indicates that programming is pending.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Security Access Denied - No More Attempts</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Access to the service is denied due to maximum retries reached.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Upload Download Not Accepted</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: The server cannot perform the requested upload or download operation.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Transfer Data Suspended</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Data transfer is temporarily suspended.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>General Data Transfer Failure</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Indicates a data transfer issue.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Data Transfer Out of Range</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: The requested data transfer is outside acceptable parameters.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Invalid Sequence</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: The sequence of commands is invalid.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Invalid Key</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: The security key provided by the client is invalid.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Exceeded Number of Attempts to Access Security</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: The client exceeded attempts for secure access.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Session Expired</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: The current session has expired.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Session Expired - Lockout Period Active</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: The session expired, and a lockout period is active.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Out of Sync</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: The communication is out of sync.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Data Transfer Error</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: There was an error during data transfer.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Transfer Data Suspended Due to Error</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Data transfer was suspended due to an error.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Transfer Data Resumed</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Data transfer has resumed.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Invalid Transfer Data</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: The data for transfer is invalid.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Reserved for Future Use</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: This code is reserved for potential future use.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Invalid Format</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Indicates an invalid message format.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Format Not Supported</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: The data format is not supported.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Transmission Error</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: There was an error during transmission.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Checksum Error</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: A checksum error was detected.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Invalid Data Length</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: The length of the data is invalid.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>CRC Error</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: A cyclic redundancy check (CRC) error occurred.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Reserved for Future Use</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Placeholder for future standard or manufacturer-defined code.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Service Not Supported in Active Diagnostic Session</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: The requested service is unavailable in the active session.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Invalid Format</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: The format of the request is invalid.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Incorrect Message Length</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: The message length is incorrect.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Checksum Mismatch</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: A checksum mismatch was detected.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Out of Memory</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: The server cannot process the request due to insufficient memory.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Memory Allocation Failure</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: The server failed to allocate memory.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Operation Timed Out</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: The operation took too long to complete.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Resource Not Available</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: A necessary resource is unavailable.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Feature Not Supported</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: The requested feature is not supported.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Unsupported Parameter</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: A parameter in the request is unsupported.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Operation Aborted</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: The operation was aborted.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Invalid Parameter</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: The parameter in the request is invalid.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Operation Failed</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: The operation failed to complete successfully.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>General Test Service</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Reserved code; generally not assigned to a specific service.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Start Diagnostic Session</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Initiates a diagnostic session.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Read DTC Information</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Retrieves Diagnostic Trouble Code (DTC) information from the ECU.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Diagnostic Session Control</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Controls the diagnostic session state.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ECU Reset</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Requests a reset of the Electronic Control Unit (ECU).</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Read Freeze Frame Data</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Reads data stored at the time of a fault occurrence.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Clear Diagnostic Information</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Clears stored diagnostic trouble codes (DTCs).</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Read Data By Identifier</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Reads data specified by an identifier.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Read Memory By Address</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Reads data from a specific memory address.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Write Data By Identifier</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Writes data to a specified identifier.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Input Output Control By Identifier</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Controls I/O functions by identifier.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Routine Control</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Controls specific diagnostic routines, such as testing or calibration.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Read Data By Periodic Identifier</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Periodically reads data using an identifier.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Read Data By Identifier</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Standard service to read data by a specific identifier.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Read Memory By Address</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Reads memory contents at a given address (similar to 0x15).</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Read Scaling Data By Identifier</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Reads scaling data, often for calibration purposes.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Security Access</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Requests access to security-protected services.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Communication Control</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Controls diagnostic communication (e.g., enabling/disabling).</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Write Data By Identifier</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Writes data specified by an identifier (similar to 0x18).</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Dynamically Define Data Identifier</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Defines a custom data identifier.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Request Download</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Requests permission to start downloading data to the ECU.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Request Upload</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Requests permission to start uploading data from the ECU.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Transfer Data</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Transfers data to/from the ECU.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Request Transfer Exit</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Ends a data transfer session.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Request File Transfer</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Manages file transfers between the client and server.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Write Data By Periodic Identifier</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Writes data periodically by identifier.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>IO Control By Identifier</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Controls input/output functions by a specified identifier.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Request Seed</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Requests a seed value for security access.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Transfer Seed</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Transfers a seed value for security access.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Check Programming Dependencies</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Verifies dependencies before programming.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Response On Event</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Enables/disables responses based on specified events.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Response Pending</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Indicates that the response is pending.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Read ECU Identification</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Reads ECU identification data.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Programming Session</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Controls the ECU programming session.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Security Access (Seed)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: An alternative security access service.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Transfer Data (Session)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Transfers data within a specific session.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Request Seed and Key</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Requests both seed and key for security access.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Write Data By Identifier</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: An additional write data service.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Read Data By Periodic Identifier</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Reads data periodically.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Tester Present</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Keeps the communication channel alive during diagnostics.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Access Timing Parameters</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Allows access to timing parameters of the ECU.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Control DTC Settings</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Controls the setting and storing of DTCs.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Clear DTC Settings</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Clears DTC settings.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Reserved for Future Use</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Placeholder for future services.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Activate Diagnostic Function</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Activates diagnostic functions in the ECU.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Deactivate Diagnostic Function</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Deactivates diagnostic functions in the ECU.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Read Data By Memory Address</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Reads data from a memory address (similar to 0x15).</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Request Upload</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Requests to upload data from the ECU.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Request Download</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Requests to download data to the ECU.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Transfer Exit</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Ends a transfer session.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Extended Data Record Information</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Accesses extended data records.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Control DTC Settings</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Configures settings for DTCs.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Reset ECU</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Resets the ECU (similar to 0x11).</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Reserved for Future Use</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Placeholder for future standard or manufacturer-defined codes.</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1108,6 +2886,14 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1133,7 +2919,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1160,6 +2946,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1497,8 +3284,8 @@
   <dimension ref="A1:D108"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C19" sqref="C19"/>
+      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:A108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3024,21 +4811,900 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16F8116D-28FC-044F-8BC7-3AC2F86422F3}">
+  <dimension ref="A1:B108"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="K24" sqref="K24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="10" t="s">
+        <v>349</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>132</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>133</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>135</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>87</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>88</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>89</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>15</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>144</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>146</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>59</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>149</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>62</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>151</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>90</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>65</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>68</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>71</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>74</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>77</v>
+      </c>
+      <c r="B37" s="10" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>91</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>157</v>
+      </c>
+      <c r="B39" s="10" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>53</v>
+      </c>
+      <c r="B40" s="10" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>18</v>
+      </c>
+      <c r="B41" s="10" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>160</v>
+      </c>
+      <c r="B42" s="10" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>161</v>
+      </c>
+      <c r="B43" s="10" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>162</v>
+      </c>
+      <c r="B44" s="10" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>163</v>
+      </c>
+      <c r="B45" s="10" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>1</v>
+      </c>
+      <c r="B46" s="10" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>4</v>
+      </c>
+      <c r="B47" s="10" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>93</v>
+      </c>
+      <c r="B48" s="10" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>94</v>
+      </c>
+      <c r="B49" s="10" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>7</v>
+      </c>
+      <c r="B50" s="10" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>95</v>
+      </c>
+      <c r="B51" s="10" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>98</v>
+      </c>
+      <c r="B52" s="10" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>57</v>
+      </c>
+      <c r="B53" s="10" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>99</v>
+      </c>
+      <c r="B54" s="10" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>169</v>
+      </c>
+      <c r="B55" s="10" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>36</v>
+      </c>
+      <c r="B56" s="10" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>39</v>
+      </c>
+      <c r="B57" s="10" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>42</v>
+      </c>
+      <c r="B58" s="10" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>173</v>
+      </c>
+      <c r="B59" s="10" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>174</v>
+      </c>
+      <c r="B60" s="10" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>10</v>
+      </c>
+      <c r="B61" s="10" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>13</v>
+      </c>
+      <c r="B62" s="10" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>16</v>
+      </c>
+      <c r="B63" s="10" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>45</v>
+      </c>
+      <c r="B64" s="10" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>179</v>
+      </c>
+      <c r="B65" s="10" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>48</v>
+      </c>
+      <c r="B66" s="10" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>181</v>
+      </c>
+      <c r="B67" s="10" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>51</v>
+      </c>
+      <c r="B68" s="10" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>60</v>
+      </c>
+      <c r="B69" s="10" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>103</v>
+      </c>
+      <c r="B70" s="10" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>63</v>
+      </c>
+      <c r="B71" s="10" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>104</v>
+      </c>
+      <c r="B72" s="10" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>105</v>
+      </c>
+      <c r="B73" s="10" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>66</v>
+      </c>
+      <c r="B74" s="10" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>69</v>
+      </c>
+      <c r="B75" s="10" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>72</v>
+      </c>
+      <c r="B76" s="10" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>75</v>
+      </c>
+      <c r="B77" s="10" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>78</v>
+      </c>
+      <c r="B78" s="10" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>190</v>
+      </c>
+      <c r="B79" s="10" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>191</v>
+      </c>
+      <c r="B80" s="10" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>54</v>
+      </c>
+      <c r="B81" s="10" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>19</v>
+      </c>
+      <c r="B82" s="10" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>80</v>
+      </c>
+      <c r="B83" s="10" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>195</v>
+      </c>
+      <c r="B84" s="10" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>107</v>
+      </c>
+      <c r="B85" s="10" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>21</v>
+      </c>
+      <c r="B86" s="10" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>23</v>
+      </c>
+      <c r="B87" s="10" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>26</v>
+      </c>
+      <c r="B88" s="10" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>29</v>
+      </c>
+      <c r="B89" s="10" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>32</v>
+      </c>
+      <c r="B90" s="10" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>108</v>
+      </c>
+      <c r="B91" s="10" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>109</v>
+      </c>
+      <c r="B92" s="10" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>200</v>
+      </c>
+      <c r="B93" s="10" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>201</v>
+      </c>
+      <c r="B94" s="10" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>204</v>
+      </c>
+      <c r="B95" s="10" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>205</v>
+      </c>
+      <c r="B96" s="10" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>206</v>
+      </c>
+      <c r="B97" s="10" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>22</v>
+      </c>
+      <c r="B98" s="10" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>24</v>
+      </c>
+      <c r="B99" s="10" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>27</v>
+      </c>
+      <c r="B100" s="10" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>30</v>
+      </c>
+      <c r="B101" s="10" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>33</v>
+      </c>
+      <c r="B102" s="10" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>211</v>
+      </c>
+      <c r="B103" s="10" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>212</v>
+      </c>
+      <c r="B104" s="10" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>213</v>
+      </c>
+      <c r="B105" s="10" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>214</v>
+      </c>
+      <c r="B106" s="10" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>216</v>
+      </c>
+      <c r="B107" s="10" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>217</v>
+      </c>
+      <c r="B108" s="10" t="s">
+        <v>468</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A03570A-127B-3341-B38D-DB2BAB5CD826}">
   <dimension ref="A1:C84"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="56.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="255.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="58.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="255.83203125" customWidth="1"/>
     <col min="4" max="4" width="169.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3058,10 +5724,10 @@
         <v>122</v>
       </c>
       <c r="B2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C2" t="s">
-        <v>218</v>
+        <v>348</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -3072,7 +5738,7 @@
         <v>123</v>
       </c>
       <c r="C3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -3083,7 +5749,7 @@
         <v>123</v>
       </c>
       <c r="C4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -3091,10 +5757,10 @@
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -3102,10 +5768,10 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C6" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -3113,10 +5779,10 @@
         <v>85</v>
       </c>
       <c r="B7" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C7" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -3124,10 +5790,10 @@
         <v>86</v>
       </c>
       <c r="B8" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C8" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -3135,10 +5801,10 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C9" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -3149,18 +5815,18 @@
         <v>123</v>
       </c>
       <c r="C10" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B11" t="s">
         <v>123</v>
       </c>
       <c r="C11" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -3168,10 +5834,10 @@
         <v>87</v>
       </c>
       <c r="B12" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C12" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -3179,10 +5845,10 @@
         <v>35</v>
       </c>
       <c r="B13" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C13" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -3193,7 +5859,7 @@
         <v>123</v>
       </c>
       <c r="C14" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -3201,10 +5867,10 @@
         <v>41</v>
       </c>
       <c r="B15" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C15" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -3212,10 +5878,10 @@
         <v>88</v>
       </c>
       <c r="B16" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C16" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -3223,10 +5889,10 @@
         <v>89</v>
       </c>
       <c r="B17" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C17" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -3237,7 +5903,7 @@
         <v>123</v>
       </c>
       <c r="C18" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -3248,7 +5914,7 @@
         <v>123</v>
       </c>
       <c r="C19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -3256,10 +5922,10 @@
         <v>62</v>
       </c>
       <c r="B20" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C20" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -3270,7 +5936,7 @@
         <v>123</v>
       </c>
       <c r="C21" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -3278,10 +5944,10 @@
         <v>90</v>
       </c>
       <c r="B22" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C22" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -3289,10 +5955,10 @@
         <v>65</v>
       </c>
       <c r="B23" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C23" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -3300,10 +5966,10 @@
         <v>68</v>
       </c>
       <c r="B24" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C24" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -3311,10 +5977,10 @@
         <v>71</v>
       </c>
       <c r="B25" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C25" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -3322,10 +5988,10 @@
         <v>74</v>
       </c>
       <c r="B26" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C26" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -3333,10 +5999,10 @@
         <v>77</v>
       </c>
       <c r="B27" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C27" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -3344,10 +6010,10 @@
         <v>91</v>
       </c>
       <c r="B28" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C28" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -3355,21 +6021,21 @@
         <v>92</v>
       </c>
       <c r="B29" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C29" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B30" t="s">
         <v>123</v>
       </c>
       <c r="C30" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -3380,7 +6046,7 @@
         <v>123</v>
       </c>
       <c r="C31" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
@@ -3388,10 +6054,10 @@
         <v>1</v>
       </c>
       <c r="B32" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C32" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
@@ -3399,10 +6065,10 @@
         <v>4</v>
       </c>
       <c r="B33" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C33" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
@@ -3410,10 +6076,10 @@
         <v>93</v>
       </c>
       <c r="B34" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C34" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
@@ -3421,10 +6087,10 @@
         <v>94</v>
       </c>
       <c r="B35" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C35" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
@@ -3432,10 +6098,10 @@
         <v>7</v>
       </c>
       <c r="B36" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C36" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
@@ -3443,10 +6109,10 @@
         <v>95</v>
       </c>
       <c r="B37" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C37" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
@@ -3454,10 +6120,10 @@
         <v>96</v>
       </c>
       <c r="B38" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C38" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
@@ -3465,10 +6131,10 @@
         <v>97</v>
       </c>
       <c r="B39" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C39" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
@@ -3476,10 +6142,10 @@
         <v>98</v>
       </c>
       <c r="B40" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C40" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
@@ -3487,10 +6153,10 @@
         <v>57</v>
       </c>
       <c r="B41" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C41" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
@@ -3498,10 +6164,10 @@
         <v>99</v>
       </c>
       <c r="B42" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C42" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
@@ -3509,10 +6175,10 @@
         <v>100</v>
       </c>
       <c r="B43" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C43" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
@@ -3520,10 +6186,10 @@
         <v>101</v>
       </c>
       <c r="B44" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C44" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
@@ -3531,21 +6197,21 @@
         <v>102</v>
       </c>
       <c r="B45" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C45" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B46" t="s">
         <v>123</v>
       </c>
       <c r="C46" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
@@ -3556,7 +6222,7 @@
         <v>123</v>
       </c>
       <c r="C47" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
@@ -3564,10 +6230,10 @@
         <v>103</v>
       </c>
       <c r="B48" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C48" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
@@ -3575,10 +6241,10 @@
         <v>63</v>
       </c>
       <c r="B49" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C49" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
@@ -3586,10 +6252,10 @@
         <v>104</v>
       </c>
       <c r="B50" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C50" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
@@ -3597,10 +6263,10 @@
         <v>105</v>
       </c>
       <c r="B51" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C51" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
@@ -3611,7 +6277,7 @@
         <v>123</v>
       </c>
       <c r="C52" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
@@ -3622,7 +6288,7 @@
         <v>123</v>
       </c>
       <c r="C53" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
@@ -3630,10 +6296,10 @@
         <v>78</v>
       </c>
       <c r="B54" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C54" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
@@ -3644,7 +6310,7 @@
         <v>123</v>
       </c>
       <c r="C55" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
@@ -3655,7 +6321,7 @@
         <v>123</v>
       </c>
       <c r="C56" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
@@ -3663,10 +6329,10 @@
         <v>19</v>
       </c>
       <c r="B57" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C57" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
@@ -3674,10 +6340,10 @@
         <v>80</v>
       </c>
       <c r="B58" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C58" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
@@ -3688,7 +6354,7 @@
         <v>123</v>
       </c>
       <c r="C59" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
@@ -3696,10 +6362,10 @@
         <v>106</v>
       </c>
       <c r="B60" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C60" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
@@ -3707,10 +6373,10 @@
         <v>107</v>
       </c>
       <c r="B61" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C61" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
@@ -3718,10 +6384,10 @@
         <v>21</v>
       </c>
       <c r="B62" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C62" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
@@ -3729,10 +6395,10 @@
         <v>23</v>
       </c>
       <c r="B63" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C63" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
@@ -3740,10 +6406,10 @@
         <v>26</v>
       </c>
       <c r="B64" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C64" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
@@ -3751,10 +6417,10 @@
         <v>29</v>
       </c>
       <c r="B65" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C65" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
@@ -3762,10 +6428,10 @@
         <v>32</v>
       </c>
       <c r="B66" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C66" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
@@ -3773,10 +6439,10 @@
         <v>108</v>
       </c>
       <c r="B67" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C67" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
@@ -3784,10 +6450,10 @@
         <v>109</v>
       </c>
       <c r="B68" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C68" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
@@ -3795,10 +6461,10 @@
         <v>110</v>
       </c>
       <c r="B69" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C69" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
@@ -3806,10 +6472,10 @@
         <v>111</v>
       </c>
       <c r="B70" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C70" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
@@ -3817,10 +6483,10 @@
         <v>112</v>
       </c>
       <c r="B71" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C71" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
@@ -3828,21 +6494,21 @@
         <v>113</v>
       </c>
       <c r="B72" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C72" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B73" t="s">
         <v>123</v>
       </c>
       <c r="C73" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
@@ -3850,10 +6516,10 @@
         <v>114</v>
       </c>
       <c r="B74" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C74" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
@@ -3861,10 +6527,10 @@
         <v>115</v>
       </c>
       <c r="B75" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C75" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
@@ -3872,10 +6538,10 @@
         <v>116</v>
       </c>
       <c r="B76" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C76" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
@@ -3883,10 +6549,10 @@
         <v>117</v>
       </c>
       <c r="B77" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C77" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
@@ -3894,10 +6560,10 @@
         <v>118</v>
       </c>
       <c r="B78" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C78" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
@@ -3905,43 +6571,43 @@
         <v>119</v>
       </c>
       <c r="B79" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C79" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
+        <v>276</v>
+      </c>
+      <c r="B80" t="s">
+        <v>342</v>
+      </c>
+      <c r="C80" t="s">
         <v>277</v>
-      </c>
-      <c r="B80" t="s">
-        <v>343</v>
-      </c>
-      <c r="C80" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B81" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C81" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
+        <v>279</v>
+      </c>
+      <c r="B82" t="s">
+        <v>343</v>
+      </c>
+      <c r="C82" t="s">
         <v>280</v>
-      </c>
-      <c r="B82" t="s">
-        <v>344</v>
-      </c>
-      <c r="C82" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
@@ -3949,10 +6615,10 @@
         <v>216</v>
       </c>
       <c r="B83" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C83" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
@@ -3963,7 +6629,686 @@
         <v>123</v>
       </c>
       <c r="C84" t="s">
-        <v>219</v>
+        <v>218</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAB86B2A-53C1-CA47-B007-ADF0BAC757ED}">
+  <dimension ref="A1:B83"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="10" t="s">
+        <v>349</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>132</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>224</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>87</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>88</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>89</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>149</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>62</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>151</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>90</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>65</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>68</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>71</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>74</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>77</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>91</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>92</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>238</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>163</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>1</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>4</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>93</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>94</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>7</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>95</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>96</v>
+      </c>
+      <c r="B37" s="10" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>97</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>98</v>
+      </c>
+      <c r="B39" s="10" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>57</v>
+      </c>
+      <c r="B40" s="10" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>99</v>
+      </c>
+      <c r="B41" s="10" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>100</v>
+      </c>
+      <c r="B42" s="10" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>101</v>
+      </c>
+      <c r="B43" s="10" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>102</v>
+      </c>
+      <c r="B44" s="10" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>252</v>
+      </c>
+      <c r="B45" s="10" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>60</v>
+      </c>
+      <c r="B46" s="10" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>103</v>
+      </c>
+      <c r="B47" s="10" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>63</v>
+      </c>
+      <c r="B48" s="10" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>104</v>
+      </c>
+      <c r="B49" s="10" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>105</v>
+      </c>
+      <c r="B50" s="10" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>66</v>
+      </c>
+      <c r="B51" s="10" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>75</v>
+      </c>
+      <c r="B52" s="10" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>78</v>
+      </c>
+      <c r="B53" s="10" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>190</v>
+      </c>
+      <c r="B54" s="10" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>54</v>
+      </c>
+      <c r="B55" s="10" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>19</v>
+      </c>
+      <c r="B56" s="10" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>80</v>
+      </c>
+      <c r="B57" s="10" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>195</v>
+      </c>
+      <c r="B58" s="10" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>106</v>
+      </c>
+      <c r="B59" s="10" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>107</v>
+      </c>
+      <c r="B60" s="10" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>21</v>
+      </c>
+      <c r="B61" s="10" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>23</v>
+      </c>
+      <c r="B62" s="10" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>26</v>
+      </c>
+      <c r="B63" s="10" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>29</v>
+      </c>
+      <c r="B64" s="10" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>32</v>
+      </c>
+      <c r="B65" s="10" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>108</v>
+      </c>
+      <c r="B66" s="10" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>109</v>
+      </c>
+      <c r="B67" s="10" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>110</v>
+      </c>
+      <c r="B68" s="10" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>111</v>
+      </c>
+      <c r="B69" s="10" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>112</v>
+      </c>
+      <c r="B70" s="10" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>113</v>
+      </c>
+      <c r="B71" s="10" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>270</v>
+      </c>
+      <c r="B72" s="10" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>114</v>
+      </c>
+      <c r="B73" s="10" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>115</v>
+      </c>
+      <c r="B74" s="10" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>116</v>
+      </c>
+      <c r="B75" s="10" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>117</v>
+      </c>
+      <c r="B76" s="10" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>118</v>
+      </c>
+      <c r="B77" s="10" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>119</v>
+      </c>
+      <c r="B78" s="10" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>276</v>
+      </c>
+      <c r="B79" s="10" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>278</v>
+      </c>
+      <c r="B80" s="10" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>279</v>
+      </c>
+      <c r="B81" s="10" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>216</v>
+      </c>
+      <c r="B82" s="10" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>217</v>
+      </c>
+      <c r="B83" s="10" t="s">
+        <v>401</v>
       </c>
     </row>
   </sheetData>

</xml_diff>